<commit_message>
Bæta við greiningu á lögregluumdæmum
</commit_message>
<xml_diff>
--- a/Data/logregla_hofudborgarsvaedis.xlsx
+++ b/Data/logregla_hofudborgarsvaedis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brynjolfurjonsson/Metill/R/logregla/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C72F0F-301C-C341-8679-08381CADDA2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07EF4B3-6BE7-D64F-90BA-E2019A333AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="20980" windowHeight="27720" xr2:uid="{1A14BB46-C427-4446-B5E7-BDD862E331E3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="21580" xr2:uid="{1A14BB46-C427-4446-B5E7-BDD862E331E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ofbeldi_samtals</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>innbrot_samtals</t>
+  </si>
+  <si>
+    <t>thjofnadur</t>
+  </si>
+  <si>
+    <t>fikniefni</t>
+  </si>
+  <si>
+    <t>fikniefni_storfelld</t>
   </si>
 </sst>
 </file>
@@ -416,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29598F60-ED63-C545-B47D-B215B30B1833}">
-  <dimension ref="A1:G132"/>
+  <dimension ref="A1:J132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="J133" sqref="J133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -427,7 +436,7 @@
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -449,8 +458,17 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2013</v>
       </c>
@@ -472,8 +490,14 @@
       <c r="G2">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>335</v>
+      </c>
+      <c r="I2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>2</v>
       </c>
@@ -492,8 +516,14 @@
       <c r="G3">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>344</v>
+      </c>
+      <c r="I3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>3</v>
       </c>
@@ -512,8 +542,14 @@
       <c r="G4">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>381</v>
+      </c>
+      <c r="I4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>4</v>
       </c>
@@ -532,8 +568,14 @@
       <c r="G5">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>409</v>
+      </c>
+      <c r="I5">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>5</v>
       </c>
@@ -552,8 +594,14 @@
       <c r="G6">
         <v>82</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>389</v>
+      </c>
+      <c r="I6">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>6</v>
       </c>
@@ -572,8 +620,14 @@
       <c r="G7">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>339</v>
+      </c>
+      <c r="I7">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>7</v>
       </c>
@@ -592,8 +646,14 @@
       <c r="G8">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>309</v>
+      </c>
+      <c r="I8">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>8</v>
       </c>
@@ -612,8 +672,14 @@
       <c r="G9">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>382</v>
+      </c>
+      <c r="I9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>9</v>
       </c>
@@ -632,8 +698,14 @@
       <c r="G10">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>326</v>
+      </c>
+      <c r="I10">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>10</v>
       </c>
@@ -652,8 +724,14 @@
       <c r="G11">
         <v>59</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <v>313</v>
+      </c>
+      <c r="I11">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>11</v>
       </c>
@@ -672,8 +750,14 @@
       <c r="G12">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12">
+        <v>295</v>
+      </c>
+      <c r="I12">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>12</v>
       </c>
@@ -692,8 +776,14 @@
       <c r="G13">
         <v>69</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13">
+        <v>270</v>
+      </c>
+      <c r="I13">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2014</v>
       </c>
@@ -715,8 +805,14 @@
       <c r="G14">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14">
+        <v>300</v>
+      </c>
+      <c r="I14">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>2</v>
       </c>
@@ -735,8 +831,14 @@
       <c r="G15">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <v>287</v>
+      </c>
+      <c r="I15">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>3</v>
       </c>
@@ -755,8 +857,14 @@
       <c r="G16">
         <v>67</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <v>313</v>
+      </c>
+      <c r="I16">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>4</v>
       </c>
@@ -775,8 +883,14 @@
       <c r="G17">
         <v>74</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17">
+        <v>285</v>
+      </c>
+      <c r="I17">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <v>5</v>
       </c>
@@ -795,8 +909,14 @@
       <c r="G18">
         <v>79</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18">
+        <v>357</v>
+      </c>
+      <c r="I18">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>6</v>
       </c>
@@ -815,8 +935,14 @@
       <c r="G19">
         <v>82</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19">
+        <v>364</v>
+      </c>
+      <c r="I19">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>7</v>
       </c>
@@ -835,8 +961,14 @@
       <c r="G20">
         <v>81</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20">
+        <v>351</v>
+      </c>
+      <c r="I20">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>8</v>
       </c>
@@ -855,8 +987,14 @@
       <c r="G21">
         <v>113</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21">
+        <v>403</v>
+      </c>
+      <c r="I21">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>9</v>
       </c>
@@ -875,8 +1013,14 @@
       <c r="G22">
         <v>66</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22">
+        <v>380</v>
+      </c>
+      <c r="I22">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
         <v>10</v>
       </c>
@@ -895,8 +1039,14 @@
       <c r="G23">
         <v>64</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23">
+        <v>331</v>
+      </c>
+      <c r="I23">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B24" s="1">
         <v>11</v>
       </c>
@@ -915,8 +1065,14 @@
       <c r="G24">
         <v>88</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24">
+        <v>328</v>
+      </c>
+      <c r="I24">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B25" s="1">
         <v>12</v>
       </c>
@@ -935,8 +1091,14 @@
       <c r="G25">
         <v>69</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25">
+        <v>262</v>
+      </c>
+      <c r="I25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2015</v>
       </c>
@@ -958,8 +1120,17 @@
       <c r="G26">
         <v>64</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26">
+        <v>277</v>
+      </c>
+      <c r="I26">
+        <v>125</v>
+      </c>
+      <c r="J26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B27" s="1">
         <v>2</v>
       </c>
@@ -975,8 +1146,17 @@
       <c r="G27">
         <v>71</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27">
+        <v>281</v>
+      </c>
+      <c r="I27">
+        <v>134</v>
+      </c>
+      <c r="J27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B28" s="1">
         <v>3</v>
       </c>
@@ -992,8 +1172,17 @@
       <c r="G28">
         <v>75</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28">
+        <v>310</v>
+      </c>
+      <c r="I28">
+        <v>116</v>
+      </c>
+      <c r="J28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B29" s="1">
         <v>4</v>
       </c>
@@ -1009,8 +1198,17 @@
       <c r="G29">
         <v>87</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29">
+        <v>413</v>
+      </c>
+      <c r="I29">
+        <v>128</v>
+      </c>
+      <c r="J29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B30" s="1">
         <v>5</v>
       </c>
@@ -1026,8 +1224,17 @@
       <c r="G30">
         <v>82</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30">
+        <v>378</v>
+      </c>
+      <c r="I30">
+        <v>119</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B31" s="1">
         <v>6</v>
       </c>
@@ -1043,8 +1250,17 @@
       <c r="G31">
         <v>98</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31">
+        <v>418</v>
+      </c>
+      <c r="I31">
+        <v>156</v>
+      </c>
+      <c r="J31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B32" s="1">
         <v>7</v>
       </c>
@@ -1060,8 +1276,17 @@
       <c r="G32">
         <v>107</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H32">
+        <v>460</v>
+      </c>
+      <c r="I32">
+        <v>105</v>
+      </c>
+      <c r="J32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B33" s="1">
         <v>8</v>
       </c>
@@ -1077,8 +1302,17 @@
       <c r="G33">
         <v>117</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33">
+        <v>467</v>
+      </c>
+      <c r="I33">
+        <v>136</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B34" s="1">
         <v>9</v>
       </c>
@@ -1094,8 +1328,17 @@
       <c r="G34">
         <v>99</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H34">
+        <v>475</v>
+      </c>
+      <c r="I34">
+        <v>109</v>
+      </c>
+      <c r="J34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B35" s="1">
         <v>10</v>
       </c>
@@ -1111,8 +1354,17 @@
       <c r="G35">
         <v>124</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H35">
+        <v>447</v>
+      </c>
+      <c r="I35">
+        <v>72</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B36" s="1">
         <v>11</v>
       </c>
@@ -1128,8 +1380,17 @@
       <c r="G36">
         <v>74</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36">
+        <v>334</v>
+      </c>
+      <c r="I36">
+        <v>77</v>
+      </c>
+      <c r="J36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B37" s="1">
         <v>12</v>
       </c>
@@ -1145,8 +1406,17 @@
       <c r="G37">
         <v>90</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37">
+        <v>307</v>
+      </c>
+      <c r="I37">
+        <v>77</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2016</v>
       </c>
@@ -1165,8 +1435,17 @@
       <c r="G38">
         <v>86</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38">
+        <v>300</v>
+      </c>
+      <c r="I38">
+        <v>122</v>
+      </c>
+      <c r="J38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B39">
         <v>2</v>
       </c>
@@ -1182,8 +1461,17 @@
       <c r="G39">
         <v>64</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39">
+        <v>263</v>
+      </c>
+      <c r="I39">
+        <v>115</v>
+      </c>
+      <c r="J39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B40">
         <v>3</v>
       </c>
@@ -1199,8 +1487,17 @@
       <c r="G40">
         <v>80</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H40">
+        <v>334</v>
+      </c>
+      <c r="I40">
+        <v>119</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B41">
         <v>4</v>
       </c>
@@ -1216,8 +1513,17 @@
       <c r="G41">
         <v>101</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41">
+        <v>362</v>
+      </c>
+      <c r="I41">
+        <v>79</v>
+      </c>
+      <c r="J41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B42">
         <v>5</v>
       </c>
@@ -1233,8 +1539,17 @@
       <c r="G42">
         <v>72</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42">
+        <v>306</v>
+      </c>
+      <c r="I42">
+        <v>121</v>
+      </c>
+      <c r="J42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B43">
         <v>6</v>
       </c>
@@ -1250,8 +1565,17 @@
       <c r="G43">
         <v>55</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H43">
+        <v>300</v>
+      </c>
+      <c r="I43">
+        <v>128</v>
+      </c>
+      <c r="J43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B44">
         <v>7</v>
       </c>
@@ -1267,8 +1591,17 @@
       <c r="G44">
         <v>63</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H44">
+        <v>327</v>
+      </c>
+      <c r="I44">
+        <v>124</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B45">
         <v>8</v>
       </c>
@@ -1284,8 +1617,17 @@
       <c r="G45">
         <v>47</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H45">
+        <v>295</v>
+      </c>
+      <c r="I45">
+        <v>108</v>
+      </c>
+      <c r="J45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>9</v>
       </c>
@@ -1301,8 +1643,17 @@
       <c r="G46">
         <v>65</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H46">
+        <v>351</v>
+      </c>
+      <c r="I46">
+        <v>139</v>
+      </c>
+      <c r="J46">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B47">
         <v>10</v>
       </c>
@@ -1318,8 +1669,17 @@
       <c r="G47">
         <v>60</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H47">
+        <v>338</v>
+      </c>
+      <c r="I47">
+        <v>100</v>
+      </c>
+      <c r="J47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B48">
         <v>11</v>
       </c>
@@ -1335,8 +1695,17 @@
       <c r="G48">
         <v>94</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48">
+        <v>310</v>
+      </c>
+      <c r="I48">
+        <v>106</v>
+      </c>
+      <c r="J48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B49">
         <v>12</v>
       </c>
@@ -1352,8 +1721,17 @@
       <c r="G49">
         <v>67</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H49">
+        <v>262</v>
+      </c>
+      <c r="I49">
+        <v>107</v>
+      </c>
+      <c r="J49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2017</v>
       </c>
@@ -1375,8 +1753,17 @@
       <c r="G50">
         <v>94</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H50">
+        <v>342</v>
+      </c>
+      <c r="I50">
+        <v>120</v>
+      </c>
+      <c r="J50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B51">
         <v>2</v>
       </c>
@@ -1395,8 +1782,17 @@
       <c r="G51">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H51">
+        <v>269</v>
+      </c>
+      <c r="I51">
+        <v>98</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B52">
         <v>3</v>
       </c>
@@ -1415,8 +1811,17 @@
       <c r="G52">
         <v>69</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H52">
+        <v>336</v>
+      </c>
+      <c r="I52">
+        <v>127</v>
+      </c>
+      <c r="J52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B53">
         <v>4</v>
       </c>
@@ -1435,8 +1840,17 @@
       <c r="G53">
         <v>90</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H53">
+        <v>322</v>
+      </c>
+      <c r="I53">
+        <v>147</v>
+      </c>
+      <c r="J53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B54">
         <v>5</v>
       </c>
@@ -1455,8 +1869,17 @@
       <c r="G54">
         <v>65</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H54">
+        <v>330</v>
+      </c>
+      <c r="I54">
+        <v>173</v>
+      </c>
+      <c r="J54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B55">
         <v>6</v>
       </c>
@@ -1475,8 +1898,17 @@
       <c r="G55">
         <v>59</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H55">
+        <v>315</v>
+      </c>
+      <c r="I55">
+        <v>188</v>
+      </c>
+      <c r="J55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B56">
         <v>7</v>
       </c>
@@ -1495,8 +1927,17 @@
       <c r="G56">
         <v>52</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H56">
+        <v>318</v>
+      </c>
+      <c r="I56">
+        <v>139</v>
+      </c>
+      <c r="J56">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B57">
         <v>8</v>
       </c>
@@ -1515,8 +1956,17 @@
       <c r="G57">
         <v>75</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H57">
+        <v>413</v>
+      </c>
+      <c r="I57">
+        <v>136</v>
+      </c>
+      <c r="J57">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B58">
         <v>9</v>
       </c>
@@ -1535,8 +1985,17 @@
       <c r="G58">
         <v>82</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H58">
+        <v>440</v>
+      </c>
+      <c r="I58">
+        <v>122</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B59">
         <v>10</v>
       </c>
@@ -1555,8 +2014,17 @@
       <c r="G59">
         <v>84</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H59">
+        <v>389</v>
+      </c>
+      <c r="I59">
+        <v>130</v>
+      </c>
+      <c r="J59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B60">
         <v>11</v>
       </c>
@@ -1575,8 +2043,17 @@
       <c r="G60">
         <v>99</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H60">
+        <v>395</v>
+      </c>
+      <c r="I60">
+        <v>140</v>
+      </c>
+      <c r="J60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B61">
         <v>12</v>
       </c>
@@ -1595,8 +2072,17 @@
       <c r="G61">
         <v>77</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H61">
+        <v>289</v>
+      </c>
+      <c r="I61">
+        <v>132</v>
+      </c>
+      <c r="J61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2018</v>
       </c>
@@ -1618,8 +2104,17 @@
       <c r="G62">
         <v>95</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H62">
+        <v>279</v>
+      </c>
+      <c r="I62">
+        <v>138</v>
+      </c>
+      <c r="J62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B63">
         <v>2</v>
       </c>
@@ -1638,8 +2133,17 @@
       <c r="G63">
         <v>98</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H63">
+        <v>280</v>
+      </c>
+      <c r="I63">
+        <v>127</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B64">
         <v>3</v>
       </c>
@@ -1658,8 +2162,17 @@
       <c r="G64">
         <v>76</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H64">
+        <v>306</v>
+      </c>
+      <c r="I64">
+        <v>181</v>
+      </c>
+      <c r="J64">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B65">
         <v>4</v>
       </c>
@@ -1678,8 +2191,17 @@
       <c r="G65">
         <v>75</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H65">
+        <v>307</v>
+      </c>
+      <c r="I65">
+        <v>141</v>
+      </c>
+      <c r="J65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B66">
         <v>5</v>
       </c>
@@ -1698,8 +2220,17 @@
       <c r="G66">
         <v>100</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H66">
+        <v>344</v>
+      </c>
+      <c r="I66">
+        <v>131</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B67">
         <v>6</v>
       </c>
@@ -1718,8 +2249,17 @@
       <c r="G67">
         <v>75</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H67">
+        <v>341</v>
+      </c>
+      <c r="I67">
+        <v>216</v>
+      </c>
+      <c r="J67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B68">
         <v>7</v>
       </c>
@@ -1738,8 +2278,17 @@
       <c r="G68">
         <v>80</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H68">
+        <v>337</v>
+      </c>
+      <c r="I68">
+        <v>127</v>
+      </c>
+      <c r="J68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B69">
         <v>8</v>
       </c>
@@ -1758,8 +2307,17 @@
       <c r="G69">
         <v>69</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H69">
+        <v>359</v>
+      </c>
+      <c r="I69">
+        <v>121</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B70">
         <v>9</v>
       </c>
@@ -1778,8 +2336,17 @@
       <c r="G70">
         <v>96</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H70">
+        <v>370</v>
+      </c>
+      <c r="I70">
+        <v>109</v>
+      </c>
+      <c r="J70">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B71">
         <v>10</v>
       </c>
@@ -1798,8 +2365,17 @@
       <c r="G71">
         <v>100</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H71">
+        <v>367</v>
+      </c>
+      <c r="I71">
+        <v>113</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B72">
         <v>11</v>
       </c>
@@ -1818,8 +2394,17 @@
       <c r="G72">
         <v>146</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H72">
+        <v>358</v>
+      </c>
+      <c r="I72">
+        <v>110</v>
+      </c>
+      <c r="J72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B73">
         <v>12</v>
       </c>
@@ -1838,8 +2423,17 @@
       <c r="G73">
         <v>126</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H73">
+        <v>312</v>
+      </c>
+      <c r="I73">
+        <v>111</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2019</v>
       </c>
@@ -1861,8 +2455,17 @@
       <c r="G74">
         <v>74</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H74">
+        <v>240</v>
+      </c>
+      <c r="I74">
+        <v>115</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B75">
         <v>2</v>
       </c>
@@ -1881,8 +2484,17 @@
       <c r="G75">
         <v>78</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H75">
+        <v>226</v>
+      </c>
+      <c r="I75">
+        <v>128</v>
+      </c>
+      <c r="J75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B76">
         <v>3</v>
       </c>
@@ -1901,8 +2513,17 @@
       <c r="G76">
         <v>65</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H76">
+        <v>311</v>
+      </c>
+      <c r="I76">
+        <v>152</v>
+      </c>
+      <c r="J76">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B77">
         <v>4</v>
       </c>
@@ -1921,8 +2542,17 @@
       <c r="G77">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H77">
+        <v>324</v>
+      </c>
+      <c r="I77">
+        <v>131</v>
+      </c>
+      <c r="J77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B78">
         <v>5</v>
       </c>
@@ -1941,8 +2571,17 @@
       <c r="G78">
         <v>71</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H78">
+        <v>348</v>
+      </c>
+      <c r="I78">
+        <v>86</v>
+      </c>
+      <c r="J78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B79">
         <v>6</v>
       </c>
@@ -1961,8 +2600,17 @@
       <c r="G79">
         <v>71</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H79">
+        <v>342</v>
+      </c>
+      <c r="I79">
+        <v>164</v>
+      </c>
+      <c r="J79">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B80">
         <v>7</v>
       </c>
@@ -1981,8 +2629,17 @@
       <c r="G80">
         <v>70</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H80">
+        <v>332</v>
+      </c>
+      <c r="I80">
+        <v>120</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B81">
         <v>8</v>
       </c>
@@ -2001,8 +2658,17 @@
       <c r="G81">
         <v>114</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H81">
+        <v>439</v>
+      </c>
+      <c r="I81">
+        <v>105</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B82">
         <v>9</v>
       </c>
@@ -2021,8 +2687,17 @@
       <c r="G82">
         <v>101</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H82">
+        <v>441</v>
+      </c>
+      <c r="I82">
+        <v>103</v>
+      </c>
+      <c r="J82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B83">
         <v>10</v>
       </c>
@@ -2041,8 +2716,17 @@
       <c r="G83">
         <v>137</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H83">
+        <v>434</v>
+      </c>
+      <c r="I83">
+        <v>117</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B84">
         <v>11</v>
       </c>
@@ -2061,8 +2745,17 @@
       <c r="G84">
         <v>95</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H84">
+        <v>350</v>
+      </c>
+      <c r="I84">
+        <v>95</v>
+      </c>
+      <c r="J84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B85">
         <v>12</v>
       </c>
@@ -2081,8 +2774,17 @@
       <c r="G85">
         <v>99</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H85">
+        <v>311</v>
+      </c>
+      <c r="I85">
+        <v>88</v>
+      </c>
+      <c r="J85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>2020</v>
       </c>
@@ -2104,8 +2806,17 @@
       <c r="G86">
         <v>55</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H86">
+        <v>283</v>
+      </c>
+      <c r="I86">
+        <v>89</v>
+      </c>
+      <c r="J86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B87">
         <v>2</v>
       </c>
@@ -2124,8 +2835,17 @@
       <c r="G87">
         <v>101</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H87">
+        <v>334</v>
+      </c>
+      <c r="I87">
+        <v>87</v>
+      </c>
+      <c r="J87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B88">
         <v>3</v>
       </c>
@@ -2144,8 +2864,17 @@
       <c r="G88">
         <v>60</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H88">
+        <v>262</v>
+      </c>
+      <c r="I88">
+        <v>85</v>
+      </c>
+      <c r="J88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B89">
         <v>4</v>
       </c>
@@ -2164,8 +2893,17 @@
       <c r="G89">
         <v>63</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H89">
+        <v>263</v>
+      </c>
+      <c r="I89">
+        <v>88</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B90">
         <v>5</v>
       </c>
@@ -2184,8 +2922,17 @@
       <c r="G90">
         <v>45</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H90">
+        <v>306</v>
+      </c>
+      <c r="I90">
+        <v>136</v>
+      </c>
+      <c r="J90">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B91">
         <v>6</v>
       </c>
@@ -2204,8 +2951,17 @@
       <c r="G91">
         <v>76</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H91">
+        <v>303</v>
+      </c>
+      <c r="I91">
+        <v>92</v>
+      </c>
+      <c r="J91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B92">
         <v>7</v>
       </c>
@@ -2224,8 +2980,17 @@
       <c r="G92">
         <v>99</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H92">
+        <v>355</v>
+      </c>
+      <c r="I92">
+        <v>114</v>
+      </c>
+      <c r="J92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B93">
         <v>8</v>
       </c>
@@ -2244,8 +3009,17 @@
       <c r="G93">
         <v>102</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H93">
+        <v>415</v>
+      </c>
+      <c r="I93">
+        <v>90</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B94">
         <v>9</v>
       </c>
@@ -2264,8 +3038,17 @@
       <c r="G94">
         <v>85</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H94">
+        <v>393</v>
+      </c>
+      <c r="I94">
+        <v>97</v>
+      </c>
+      <c r="J94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B95">
         <v>10</v>
       </c>
@@ -2284,8 +3067,17 @@
       <c r="G95">
         <v>81</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H95">
+        <v>411</v>
+      </c>
+      <c r="I95">
+        <v>82</v>
+      </c>
+      <c r="J95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B96">
         <v>11</v>
       </c>
@@ -2304,8 +3096,17 @@
       <c r="G96">
         <v>59</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H96">
+        <v>320</v>
+      </c>
+      <c r="I96">
+        <v>79</v>
+      </c>
+      <c r="J96">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B97">
         <v>12</v>
       </c>
@@ -2324,8 +3125,17 @@
       <c r="G97">
         <v>84</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H97">
+        <v>287</v>
+      </c>
+      <c r="I97">
+        <v>90</v>
+      </c>
+      <c r="J97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>2021</v>
       </c>
@@ -2347,8 +3157,17 @@
       <c r="G98">
         <v>64</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H98">
+        <v>249</v>
+      </c>
+      <c r="I98">
+        <v>91</v>
+      </c>
+      <c r="J98">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B99" s="1">
         <v>2</v>
       </c>
@@ -2367,8 +3186,17 @@
       <c r="G99">
         <v>44</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H99">
+        <v>239</v>
+      </c>
+      <c r="I99">
+        <v>141</v>
+      </c>
+      <c r="J99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B100" s="1">
         <v>3</v>
       </c>
@@ -2387,8 +3215,17 @@
       <c r="G100">
         <v>36</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H100">
+        <v>294</v>
+      </c>
+      <c r="I100">
+        <v>143</v>
+      </c>
+      <c r="J100">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B101" s="1">
         <v>4</v>
       </c>
@@ -2407,8 +3244,17 @@
       <c r="G101">
         <v>88</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H101">
+        <v>367</v>
+      </c>
+      <c r="I101">
+        <v>86</v>
+      </c>
+      <c r="J101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B102" s="1">
         <v>5</v>
       </c>
@@ -2427,8 +3273,17 @@
       <c r="G102">
         <v>93</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H102">
+        <v>448</v>
+      </c>
+      <c r="I102">
+        <v>115</v>
+      </c>
+      <c r="J102">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B103" s="1">
         <v>6</v>
       </c>
@@ -2447,8 +3302,17 @@
       <c r="G103">
         <v>115</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H103">
+        <v>495</v>
+      </c>
+      <c r="I103">
+        <v>85</v>
+      </c>
+      <c r="J103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B104" s="1">
         <v>7</v>
       </c>
@@ -2467,8 +3331,17 @@
       <c r="G104">
         <v>110</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H104">
+        <v>483</v>
+      </c>
+      <c r="I104">
+        <v>80</v>
+      </c>
+      <c r="J104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B105" s="1">
         <v>8</v>
       </c>
@@ -2487,8 +3360,17 @@
       <c r="G105">
         <v>83</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H105">
+        <v>372</v>
+      </c>
+      <c r="I105">
+        <v>77</v>
+      </c>
+      <c r="J105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B106" s="1">
         <v>9</v>
       </c>
@@ -2507,8 +3389,17 @@
       <c r="G106">
         <v>86</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H106">
+        <v>391</v>
+      </c>
+      <c r="I106">
+        <v>91</v>
+      </c>
+      <c r="J106">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B107" s="1">
         <v>10</v>
       </c>
@@ -2527,8 +3418,17 @@
       <c r="G107">
         <v>86</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H107">
+        <v>404</v>
+      </c>
+      <c r="I107">
+        <v>93</v>
+      </c>
+      <c r="J107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B108" s="1">
         <v>11</v>
       </c>
@@ -2547,8 +3447,17 @@
       <c r="G108">
         <v>58</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H108">
+        <v>262</v>
+      </c>
+      <c r="I108">
+        <v>59</v>
+      </c>
+      <c r="J108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B109" s="1">
         <v>12</v>
       </c>
@@ -2567,8 +3476,17 @@
       <c r="G109">
         <v>64</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H109">
+        <v>297</v>
+      </c>
+      <c r="I109">
+        <v>74</v>
+      </c>
+      <c r="J109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>2022</v>
       </c>
@@ -2590,8 +3508,17 @@
       <c r="G110">
         <v>66</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H110">
+        <v>255</v>
+      </c>
+      <c r="I110">
+        <v>85</v>
+      </c>
+      <c r="J110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B111" s="1">
         <v>2</v>
       </c>
@@ -2610,8 +3537,17 @@
       <c r="G111">
         <v>47</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H111">
+        <v>212</v>
+      </c>
+      <c r="I111">
+        <v>76</v>
+      </c>
+      <c r="J111">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B112" s="1">
         <v>3</v>
       </c>
@@ -2630,8 +3566,17 @@
       <c r="G112">
         <v>65</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H112">
+        <v>313</v>
+      </c>
+      <c r="I112">
+        <v>83</v>
+      </c>
+      <c r="J112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B113" s="1">
         <v>4</v>
       </c>
@@ -2650,8 +3595,17 @@
       <c r="G113">
         <v>69</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H113">
+        <v>274</v>
+      </c>
+      <c r="I113">
+        <v>90</v>
+      </c>
+      <c r="J113">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B114" s="1">
         <v>5</v>
       </c>
@@ -2670,8 +3624,17 @@
       <c r="G114">
         <v>65</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H114">
+        <v>310</v>
+      </c>
+      <c r="I114">
+        <v>117</v>
+      </c>
+      <c r="J114">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B115" s="1">
         <v>6</v>
       </c>
@@ -2690,8 +3653,17 @@
       <c r="G115">
         <v>107</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H115">
+        <v>378</v>
+      </c>
+      <c r="I115">
+        <v>100</v>
+      </c>
+      <c r="J115">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B116" s="1">
         <v>7</v>
       </c>
@@ -2710,8 +3682,17 @@
       <c r="G116">
         <v>92</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H116">
+        <v>379</v>
+      </c>
+      <c r="I116">
+        <v>75</v>
+      </c>
+      <c r="J116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B117" s="1">
         <v>8</v>
       </c>
@@ -2730,8 +3711,17 @@
       <c r="G117">
         <v>127</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H117">
+        <v>455</v>
+      </c>
+      <c r="I117">
+        <v>93</v>
+      </c>
+      <c r="J117">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B118" s="1">
         <v>9</v>
       </c>
@@ -2750,8 +3740,17 @@
       <c r="G118">
         <v>102</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H118">
+        <v>416</v>
+      </c>
+      <c r="I118">
+        <v>82</v>
+      </c>
+      <c r="J118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B119" s="1">
         <v>10</v>
       </c>
@@ -2770,8 +3769,17 @@
       <c r="G119">
         <v>107</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H119">
+        <v>407</v>
+      </c>
+      <c r="I119">
+        <v>96</v>
+      </c>
+      <c r="J119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B120" s="1">
         <v>11</v>
       </c>
@@ -2790,8 +3798,17 @@
       <c r="G120">
         <v>85</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H120">
+        <v>311</v>
+      </c>
+      <c r="I120">
+        <v>112</v>
+      </c>
+      <c r="J120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B121" s="1">
         <v>12</v>
       </c>
@@ -2810,8 +3827,17 @@
       <c r="G121">
         <v>53</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H121">
+        <v>227</v>
+      </c>
+      <c r="I121">
+        <v>80</v>
+      </c>
+      <c r="J121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>2023</v>
       </c>
@@ -2833,8 +3859,17 @@
       <c r="G122">
         <v>81</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H122">
+        <v>267</v>
+      </c>
+      <c r="I122">
+        <v>54</v>
+      </c>
+      <c r="J122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B123" s="1">
         <v>2</v>
       </c>
@@ -2853,8 +3888,17 @@
       <c r="G123">
         <v>65</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H123">
+        <v>269</v>
+      </c>
+      <c r="I123">
+        <v>86</v>
+      </c>
+      <c r="J123">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B124" s="1">
         <v>3</v>
       </c>
@@ -2873,8 +3917,17 @@
       <c r="G124">
         <v>78</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H124">
+        <v>338</v>
+      </c>
+      <c r="I124">
+        <v>76</v>
+      </c>
+      <c r="J124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B125" s="1">
         <v>4</v>
       </c>
@@ -2893,8 +3946,17 @@
       <c r="G125">
         <v>91</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H125">
+        <v>355</v>
+      </c>
+      <c r="I125">
+        <v>82</v>
+      </c>
+      <c r="J125">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B126" s="1">
         <v>5</v>
       </c>
@@ -2913,8 +3975,17 @@
       <c r="G126">
         <v>59</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H126">
+        <v>297</v>
+      </c>
+      <c r="I126">
+        <v>65</v>
+      </c>
+      <c r="J126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B127" s="1">
         <v>6</v>
       </c>
@@ -2933,8 +4004,17 @@
       <c r="G127">
         <v>64</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H127">
+        <v>362</v>
+      </c>
+      <c r="I127">
+        <v>88</v>
+      </c>
+      <c r="J127">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B128" s="1">
         <v>7</v>
       </c>
@@ -2953,8 +4033,17 @@
       <c r="G128">
         <v>126</v>
       </c>
-    </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H128">
+        <v>462</v>
+      </c>
+      <c r="I128">
+        <v>94</v>
+      </c>
+      <c r="J128">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B129" s="1">
         <v>8</v>
       </c>
@@ -2973,8 +4062,17 @@
       <c r="G129">
         <v>76</v>
       </c>
-    </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H129">
+        <v>383</v>
+      </c>
+      <c r="I129">
+        <v>60</v>
+      </c>
+      <c r="J129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B130" s="1">
         <v>9</v>
       </c>
@@ -2993,8 +4091,17 @@
       <c r="G130">
         <v>59</v>
       </c>
-    </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H130">
+        <v>317</v>
+      </c>
+      <c r="I130">
+        <v>59</v>
+      </c>
+      <c r="J130">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B131" s="1">
         <v>10</v>
       </c>
@@ -3013,8 +4120,17 @@
       <c r="G131">
         <v>65</v>
       </c>
-    </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H131">
+        <v>365</v>
+      </c>
+      <c r="I131">
+        <v>77</v>
+      </c>
+      <c r="J131">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B132" s="1">
         <v>11</v>
       </c>
@@ -3032,6 +4148,15 @@
       </c>
       <c r="G132">
         <v>42</v>
+      </c>
+      <c r="H132">
+        <v>273</v>
+      </c>
+      <c r="I132">
+        <v>74</v>
+      </c>
+      <c r="J132">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>